<commit_message>
use mem_cache as s3 fallback
</commit_message>
<xml_diff>
--- a/excels/A.xlsx
+++ b/excels/A.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Doo</t>
   </si>
   <si>
-    <t xml:space="preserve">Not matched A</t>
+    <t xml:space="preserve">Dummy_A</t>
   </si>
 </sst>
 </file>
@@ -240,7 +240,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>